<commit_message>
- Changed MCU.. - Deleted unnecessary components.. - Regenerated output files.. - Updated BOM.. - Updated Batch_4_21 on google docs..
</commit_message>
<xml_diff>
--- a/X16R60/Release/BOM/X16R60.xlsx
+++ b/X16R60/Release/BOM/X16R60.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Qty</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>Vishay</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -115,49 +112,7 @@
     <t>Tolerance</t>
   </si>
   <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
     <t>100nF</t>
-  </si>
-  <si>
-    <t>C3, C5, C7, C12, C13, C14, C15, C16</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>C4, C6</t>
-  </si>
-  <si>
-    <t>22pF</t>
-  </si>
-  <si>
-    <t>C1, C2</t>
-  </si>
-  <si>
-    <t>D1, D2</t>
-  </si>
-  <si>
-    <t>VLMB1500-GS08</t>
-  </si>
-  <si>
-    <t>LED Uni-Color Blue 468nm 2-Pin Chip 0402(1006Metric) T/R</t>
-  </si>
-  <si>
-    <t>Blue LED</t>
-  </si>
-  <si>
-    <t>https://octopart.com/vlmb1500-gs08-vishay-24098162?r=sp</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>Diode</t>
-  </si>
-  <si>
-    <t>R4, R6, R13, R24, R25</t>
   </si>
   <si>
     <t>General Purpose Chip Resistor Thick Film 0402 510kOhm 1% Paper T/R</t>
@@ -183,152 +138,9 @@
     </r>
   </si>
   <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R5</t>
-  </si>
-  <si>
-    <t>Res General Purpose Thick Film 0402 47.5K Ohm 1% 1/16W ±100ppm/°C Molded SMD Paper T/R</t>
-  </si>
-  <si>
     <t>33.0R</t>
   </si>
   <si>
-    <t>R7, R8, R9, R10, R14, R16, R17, R18, R19, R20, R21, R22, R26</t>
-  </si>
-  <si>
-    <t>680.0R</t>
-  </si>
-  <si>
-    <t>R11, R15</t>
-  </si>
-  <si>
-    <t>RC0402JR-07680RL</t>
-  </si>
-  <si>
-    <t>Res General Purpose Thick Film 0402 680 Ohm 5% 1/16W ±100ppm/°C Molded SMD Paper T/R</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>±5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>%</t>
-    </r>
-  </si>
-  <si>
-    <t>https://octopart.com/rc0402jr-07680rl-yageo-40952767?r=sp</t>
-  </si>
-  <si>
-    <t>1.0M</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0402 1M Ohm 0.1% 1/16W ±50ppm/°C Molded SMD Paper T/R</t>
-  </si>
-  <si>
-    <t>RE0402BRE071ML</t>
-  </si>
-  <si>
-    <t>https://octopart.com/re0402bre071ml-yageo-71389891?r=sp</t>
-  </si>
-  <si>
-    <t>Q1, Q2</t>
-  </si>
-  <si>
-    <t>Transistors Mosfet N-channel</t>
-  </si>
-  <si>
-    <t>STM32F103C8T6</t>
-  </si>
-  <si>
-    <t>ARM Cortex-M3 STM32 F1 Microcontroller 32-Bit 72MHz 64kB FLASH LQFP48</t>
-  </si>
-  <si>
-    <t>https://octopart.com/stm32f103c8t6-stmicroelectronics-41858015?r=sp</t>
-  </si>
-  <si>
-    <t>LDO Regulator</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>LDO Regulator Pos 3.3V 0.2A 3-Pin SOT-23 Embossed T/R</t>
-  </si>
-  <si>
-    <t>Torex</t>
-  </si>
-  <si>
-    <t>XC6206P332MR-G</t>
-  </si>
-  <si>
-    <t>https://octopart.com/xc6206p332mr-g-torex-22094979?r=sp</t>
-  </si>
-  <si>
-    <t>Aker Technology USA</t>
-  </si>
-  <si>
-    <t>C7S-8.000-18-3030-X-CT</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>8MHz ±30ppm Crystal 18pF 70 Ohms 4-SMD, No Lead</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/aker-technology-usa/C7S-8-000-18-3030-X-CT/13252477</t>
-  </si>
-  <si>
-    <t>CRYSTAL 8MHZ 18PF SMD</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>Seeed Technology Co., Ltd</t>
-  </si>
-  <si>
-    <t>GROVE 4PIN CABLES 5PACK 50CM</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/seeed-technology-co.,-ltd/110990038/5482566?utm_adgroup=Accessories&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Development%20Boards%2C%20Kits%2C%20Programmers_NEW&amp;utm_term=&amp;utm_content=Accessories&amp;gclid=EAIaIQobChMI47PRw4Pu7QIVh6eGCh2HeAMtEAQYASABEgJ6jvD_BwE</t>
-  </si>
-  <si>
-    <t>K1</t>
-  </si>
-  <si>
-    <t>C&amp;K Components</t>
-  </si>
-  <si>
-    <t>Button</t>
-  </si>
-  <si>
-    <t>Y78B21110FP</t>
-  </si>
-  <si>
-    <t>https://octopart.com/y78b21110fp-c%26k+components-7269758?r=sp</t>
-  </si>
-  <si>
-    <t>Switch Tactile N.O. SPST Button Gull Wing 0.05A 32VDC 1VA 200000Cycle 1.2N SMD T/R</t>
-  </si>
-  <si>
     <t xml:space="preserve">2.54mm Straight 2X8p 16pin Box Header </t>
   </si>
   <si>
@@ -362,15 +174,6 @@
     <t>https://octopart.com/kae02lggr-e-switch-24959047?r=sp</t>
   </si>
   <si>
-    <t>Cap Ceramic 22pF 50V C0G 5% Pad SMD 0402 125C Automotive T/R</t>
-  </si>
-  <si>
-    <t>GRT1555C1H220JA02D</t>
-  </si>
-  <si>
-    <t>https://octopart.com/grt1555c1h220ja02d-murata-76357113?r=sp</t>
-  </si>
-  <si>
     <t>Cap Ceramic 0.1uF 16V X7R 20% Pad SMD 0402 125C Automotive T/R</t>
   </si>
   <si>
@@ -380,30 +183,12 @@
     <t>https://octopart.com/c0402c104k4raltu-kemet-9144042?r=sp</t>
   </si>
   <si>
-    <t>https://octopart.com/rc0402fr-074k7l-yageo-42471327?r=sp</t>
-  </si>
-  <si>
-    <t>RC0402FR-074K7L</t>
-  </si>
-  <si>
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
     <t>https://octopart.com/rc0402fr-0710kl-yageo-55458461?r=sp</t>
   </si>
   <si>
-    <t>10µF ±20% 10V Ceramic Capacitor X5R 0402 (1005 Metric)</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
-    <t>CL05A106MP5NUNC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/en/samsung-electro-mechanics/CL05A106MP5NUNC/1276-1450-2-ND/3887108</t>
-  </si>
-  <si>
     <t>33 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200 Thick Film</t>
   </si>
   <si>
@@ -419,25 +204,34 @@
     <t>https://www.digikey.de/product-detail/en/stackpole-electronics-inc/RMCF0402FT33R0/RMCF0402FT33R0TR-ND/1761476</t>
   </si>
   <si>
-    <t>Transistor MOSFET Negative Channel 100 Volt 0.17A 3-Pin SOT-23</t>
-  </si>
-  <si>
-    <t>BSS123</t>
-  </si>
-  <si>
-    <t>https://octopart.com/bss123-on+semiconductor-20837328?r=sp</t>
-  </si>
-  <si>
-    <t>Diode Schottky 40V 1A Surface Mount SMA (DO-214AC)</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>STPS140A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.de/product-detail/en/stmicroelectronics/STPS140A/497-2453-2-ND/603478</t>
+    <t>R7, R8, R9, R10, R14, R16, R17, R18, R19, R20, R21, R22</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
+  </si>
+  <si>
+    <t>C12, C13, C14, C15, C16</t>
+  </si>
+  <si>
+    <t>STM32F091CBU6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32f091cbu6-stmicroelectronics-51988677?r=sp</t>
+  </si>
+  <si>
+    <t>MCU 32-bit ARM Cortex M0 RISC 128KB Flash 2.5V/3.3V 48-Pin UFQFPN EP Frame</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>CSTNE8M00G550000R0</t>
+  </si>
+  <si>
+    <t>Ceramic Resonator 8MHz ±0.5% (Tol) ±0.2% (Stability) 33pF 40Ohm 3-Pin CSMD T/R</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cstne8m00g550000r0-murata-91406934?r=sp</t>
   </si>
 </sst>
 </file>
@@ -515,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -537,9 +331,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -850,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +665,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -889,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
@@ -900,74 +691,72 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="5" t="s">
-        <v>91</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>98</v>
+        <v>24</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="5" t="s">
-        <v>88</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -975,47 +764,51 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="H5" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>37</v>
+      </c>
       <c r="H6" s="5" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1023,23 +816,23 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="5" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1047,311 +840,34 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>74</v>
+        <v>45</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="8">
-        <v>110990038</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>5</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>2</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" display="https://octopart.com/grm21bc81e475ka12l-murata-10331911?r=sp&amp;s=RY3qZSD8T6mG6TC9CHI5qQ"/>
-    <hyperlink ref="H5" r:id="rId2" display="https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp&amp;s=_gcP4_q8T1SC6PJQPTQ9yA"/>
-    <hyperlink ref="H12" r:id="rId3"/>
-    <hyperlink ref="H14" r:id="rId4" display="https://octopart.com/crcw060310r0fkeb-vishay-42507905"/>
-    <hyperlink ref="H11" r:id="rId5"/>
-    <hyperlink ref="H3" r:id="rId6"/>
-    <hyperlink ref="H13" r:id="rId7"/>
-    <hyperlink ref="H16" r:id="rId8"/>
-    <hyperlink ref="H7" r:id="rId9"/>
-    <hyperlink ref="H6" r:id="rId10"/>
+    <hyperlink ref="H5" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId4"/>
+    <hyperlink ref="H8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>